<commit_message>
Adding to datasheet unittest, added data export class
</commit_message>
<xml_diff>
--- a/support/test_REPORT01.xlsx
+++ b/support/test_REPORT01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ErinBryson\PycharmProjects\robs_data_collector\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1F4BAE-C0F9-41CF-84CD-8D55F7E769BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F8E25D-BF85-4986-96B1-0CD0488834E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8527179C-6205-4C3F-833E-A03D9A1F4139}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8527179C-6205-4C3F-833E-A03D9A1F4139}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>NumSignals</t>
   </si>
   <si>
-    <t>TEST_ACQ_METH_NM</t>
-  </si>
-  <si>
     <t>TEST_ACQ_OP_NM</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>HeaderName</t>
+  </si>
+  <si>
+    <t>TEST_ACQ_MTH_NM</t>
   </si>
 </sst>
 </file>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E225B12-3C5C-44B7-BE8C-9B1911C35767}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +831,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E4C098-06BE-4EC4-B912-00BE409E4344}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -973,75 +973,75 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1">
         <v>8</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1">
         <v>20</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" s="1">
         <v>115.5</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N5" s="1">
         <v>6</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N6" s="1">
         <v>0.9</v>
@@ -1270,10 +1270,10 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N7" s="1">
         <v>832.4</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -1332,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N8" s="1">
         <v>0.5</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N9" s="1">
         <v>0.5</v>
@@ -1411,34 +1411,34 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>